<commit_message>
Resolved issue with HAST not correctly saving load flow settings that was run as part of the HAST run.
Also improved testing and error reporting + some code tidying
</commit_message>
<xml_diff>
--- a/hast2_1/tests/HAST_Inputs_stage_all.xlsx
+++ b/hast2_1/tests/HAST_Inputs_stage_all.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD9B8EB-A79F-4E08-BC99-150277FC5A15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09DCA75-BDC7-43A3-9380-13A4599CB576}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -2173,8 +2173,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,7 +2348,7 @@
         <v>232</v>
       </c>
       <c r="B17" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>242</v>
@@ -6271,7 +6271,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -9763,6 +9763,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -9771,15 +9780,6 @@
     <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9801,6 +9801,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9814,12 +9822,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>